<commit_message>
7. Hafta Bütçe Güncellemesi
7. Hafta için bütçe güncellemesi yapılmıştır.
</commit_message>
<xml_diff>
--- a/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
+++ b/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
@@ -635,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -809,10 +809,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -821,30 +827,24 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="30"/>
     </xf>
@@ -858,6 +858,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1389,8 +1392,8 @@
   </sheetPr>
   <dimension ref="A3:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,11 +1450,11 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="H17" s="65" t="s">
+      <c r="H17" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="66"/>
-      <c r="J17" s="67"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="72"/>
     </row>
     <row r="18" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="H18" s="45" t="s">
@@ -1531,36 +1534,36 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="68" t="s">
+      <c r="A30" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="70" t="s">
+      <c r="C30" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="63" t="s">
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="70" t="s">
+      <c r="K30" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="L30" s="71"/>
-      <c r="M30" s="71"/>
-      <c r="N30" s="63" t="s">
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="O30" s="63" t="s">
+      <c r="O30" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="P30" s="63" t="s">
+      <c r="P30" s="65" t="s">
         <v>35</v>
       </c>
       <c r="Q30" s="9" t="s">
@@ -1568,8 +1571,8 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="69"/>
-      <c r="B31" s="72"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="8" t="s">
         <v>3</v>
       </c>
@@ -1591,7 +1594,7 @@
       <c r="I31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="64"/>
+      <c r="J31" s="66"/>
       <c r="K31" s="8" t="s">
         <v>7</v>
       </c>
@@ -1601,9 +1604,9 @@
       <c r="M31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="64"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="64"/>
+      <c r="N31" s="66"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="66"/>
       <c r="Q31" s="5">
         <v>100000</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="3">
-        <f>SUM(C32:I32)</f>
+        <f t="shared" ref="J32:J38" si="0">SUM(C32:I32)</f>
         <v>34000</v>
       </c>
       <c r="K32" s="3">
@@ -1694,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="4">
-        <f>SUM(C33:I33)</f>
+        <f t="shared" si="0"/>
         <v>34000</v>
       </c>
       <c r="K33" s="4">
@@ -1751,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="3">
-        <f>SUM(C34:I34)</f>
+        <f t="shared" si="0"/>
         <v>34000</v>
       </c>
       <c r="K34" s="3">
@@ -1808,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4">
-        <f>SUM(C35:I35)</f>
+        <f t="shared" si="0"/>
         <v>34000</v>
       </c>
       <c r="K35" s="4">
@@ -1866,7 +1869,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="3">
-        <f>SUM(C36:I36)</f>
+        <f t="shared" si="0"/>
         <v>34000</v>
       </c>
       <c r="K36" s="3">
@@ -1924,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4">
-        <f>SUM(C37:I37)</f>
+        <f t="shared" si="0"/>
         <v>34000</v>
       </c>
       <c r="K37" s="4">
@@ -1960,21 +1963,56 @@
       <c r="B38" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="12"/>
+      <c r="C38" s="11">
+        <v>10000</v>
+      </c>
+      <c r="D38" s="11">
+        <v>6000</v>
+      </c>
+      <c r="E38" s="11">
+        <v>6000</v>
+      </c>
+      <c r="F38" s="11">
+        <v>4000</v>
+      </c>
+      <c r="G38" s="11">
+        <v>4000</v>
+      </c>
+      <c r="H38" s="11">
+        <v>4000</v>
+      </c>
+      <c r="I38" s="11">
+        <v>0</v>
+      </c>
+      <c r="J38" s="11">
+        <f t="shared" si="0"/>
+        <v>34000</v>
+      </c>
+      <c r="K38" s="11">
+        <v>0</v>
+      </c>
+      <c r="L38" s="11">
+        <v>0</v>
+      </c>
+      <c r="M38" s="11">
+        <v>0</v>
+      </c>
+      <c r="N38" s="11">
+        <f xml:space="preserve"> ( (M38 * L38) * K38 / 100 ) + K38</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="11">
+        <f>N38 - J38</f>
+        <v>-34000</v>
+      </c>
+      <c r="P38" s="11">
+        <f>Q38 * 0.1</f>
+        <v>12691.900000000001</v>
+      </c>
+      <c r="Q38" s="78">
+        <f xml:space="preserve"> (Q37 + O38) + P37</f>
+        <v>126919</v>
+      </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="51">
@@ -2128,7 +2166,7 @@
       <c r="I45" s="49"/>
       <c r="J45" s="49">
         <f>SUM(J32:J38)</f>
-        <v>204000</v>
+        <v>238000</v>
       </c>
       <c r="K45" s="49"/>
       <c r="L45" s="49"/>
@@ -2140,11 +2178,11 @@
       <c r="O45" s="49"/>
       <c r="P45" s="49">
         <f>SUM(P32:P44) - P36</f>
-        <v>23529</v>
+        <v>36220.9</v>
       </c>
       <c r="Q45" s="50">
-        <f xml:space="preserve"> Q37</f>
-        <v>146290</v>
+        <f xml:space="preserve"> Q38</f>
+        <v>126919</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
@@ -2160,12 +2198,12 @@
       <c r="F47" s="30"/>
     </row>
     <row r="51" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G51" s="61" t="s">
+      <c r="G51" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="H51" s="62"/>
-      <c r="I51" s="62"/>
-      <c r="J51" s="62"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="69"/>
+      <c r="J51" s="69"/>
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G52" s="13" t="s">
@@ -2201,7 +2239,7 @@
         <v>2</v>
       </c>
       <c r="H54" s="56">
-        <f t="shared" ref="H54" si="0">DATE(2015,3,18)</f>
+        <f t="shared" ref="H54" si="1">DATE(2015,3,18)</f>
         <v>42081</v>
       </c>
       <c r="I54" s="13">
@@ -2228,16 +2266,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="P30:P31"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="C30:I30"/>
     <mergeCell ref="J30:J31"/>
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="P30:P31"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -2310,34 +2348,34 @@
       </c>
       <c r="M9" s="31">
         <f ca="1">TODAY()</f>
-        <v>42098</v>
+        <v>42104</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="63" t="s">
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="70" t="s">
+      <c r="J14" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="71"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="63" t="s">
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="63" t="s">
+      <c r="N14" s="65" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="9" t="s">
@@ -2367,7 +2405,7 @@
       <c r="H15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="72"/>
+      <c r="I15" s="67"/>
       <c r="J15" s="8" t="s">
         <v>7</v>
       </c>
@@ -2377,7 +2415,7 @@
       <c r="L15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="72"/>
+      <c r="M15" s="67"/>
       <c r="N15" s="75"/>
       <c r="O15" s="5">
         <v>100000</v>
@@ -2592,7 +2630,7 @@
       <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="71"/>
+      <c r="B1" s="64"/>
       <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
8. Hafta Bütçe Güncellemesi
8. hafta için bütçe güncellemesi yapılmıştır.
</commit_message>
<xml_diff>
--- a/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
+++ b/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
@@ -635,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -809,6 +809,30 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
@@ -821,30 +845,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="30"/>
     </xf>
@@ -860,7 +863,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1392,8 +1398,8 @@
   </sheetPr>
   <dimension ref="A3:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1445,16 +1451,16 @@
         <v>31</v>
       </c>
       <c r="N9" s="31">
-        <f>DATE(2015,4,3)</f>
-        <v>42097</v>
+        <f>DATE(2015,4,17)</f>
+        <v>42111</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="H17" s="70" t="s">
+      <c r="H17" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="71"/>
-      <c r="J17" s="72"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="68"/>
     </row>
     <row r="18" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="H18" s="45" t="s">
@@ -1534,36 +1540,36 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="61" t="s">
+      <c r="A30" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="65" t="s">
+      <c r="B30" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="65" t="s">
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="63" t="s">
+      <c r="K30" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="65" t="s">
+      <c r="L30" s="72"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="O30" s="65" t="s">
+      <c r="O30" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="P30" s="65" t="s">
+      <c r="P30" s="64" t="s">
         <v>35</v>
       </c>
       <c r="Q30" s="9" t="s">
@@ -1571,8 +1577,8 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="62"/>
-      <c r="B31" s="67"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="8" t="s">
         <v>3</v>
       </c>
@@ -1594,7 +1600,7 @@
       <c r="I31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="66"/>
+      <c r="J31" s="65"/>
       <c r="K31" s="8" t="s">
         <v>7</v>
       </c>
@@ -1604,9 +1610,9 @@
       <c r="M31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="66"/>
-      <c r="O31" s="66"/>
-      <c r="P31" s="66"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
+      <c r="P31" s="65"/>
       <c r="Q31" s="5">
         <v>100000</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" ref="J32:J38" si="0">SUM(C32:I32)</f>
+        <f t="shared" ref="J32:J39" si="0">SUM(C32:I32)</f>
         <v>34000</v>
       </c>
       <c r="K32" s="3">
@@ -1943,7 +1949,7 @@
         <f xml:space="preserve"> ( (M37 * L37) * K37 / 100 ) + K37</f>
         <v>110000</v>
       </c>
-      <c r="O37" s="4">
+      <c r="O37" s="55">
         <f>N37 - J37</f>
         <v>76000</v>
       </c>
@@ -2001,7 +2007,7 @@
         <f xml:space="preserve"> ( (M38 * L38) * K38 / 100 ) + K38</f>
         <v>0</v>
       </c>
-      <c r="O38" s="11">
+      <c r="O38" s="79">
         <f>N38 - J38</f>
         <v>-34000</v>
       </c>
@@ -2009,7 +2015,7 @@
         <f>Q38 * 0.1</f>
         <v>12691.900000000001</v>
       </c>
-      <c r="Q38" s="78">
+      <c r="Q38" s="61">
         <f xml:space="preserve"> (Q37 + O38) + P37</f>
         <v>126919</v>
       </c>
@@ -2021,21 +2027,56 @@
       <c r="B39" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="52"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="52"/>
-      <c r="O39" s="52"/>
-      <c r="P39" s="52"/>
-      <c r="Q39" s="53"/>
+      <c r="C39" s="52">
+        <v>10000</v>
+      </c>
+      <c r="D39" s="52">
+        <v>6000</v>
+      </c>
+      <c r="E39" s="52">
+        <v>6000</v>
+      </c>
+      <c r="F39" s="52">
+        <v>4000</v>
+      </c>
+      <c r="G39" s="52">
+        <v>4000</v>
+      </c>
+      <c r="H39" s="52">
+        <v>4000</v>
+      </c>
+      <c r="I39" s="52">
+        <v>0</v>
+      </c>
+      <c r="J39" s="52">
+        <f t="shared" si="0"/>
+        <v>34000</v>
+      </c>
+      <c r="K39" s="52">
+        <v>0</v>
+      </c>
+      <c r="L39" s="52">
+        <v>0</v>
+      </c>
+      <c r="M39" s="52">
+        <v>0</v>
+      </c>
+      <c r="N39" s="52">
+        <f xml:space="preserve"> ( (M39 * L39) * K39 / 100 ) + K39</f>
+        <v>0</v>
+      </c>
+      <c r="O39" s="80">
+        <f>N39 - J39</f>
+        <v>-34000</v>
+      </c>
+      <c r="P39" s="52">
+        <f>Q39 * 0.1</f>
+        <v>10561.09</v>
+      </c>
+      <c r="Q39" s="53">
+        <f xml:space="preserve"> (Q38 + O39) + P38</f>
+        <v>105610.9</v>
+      </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
@@ -2165,24 +2206,24 @@
       <c r="H45" s="49"/>
       <c r="I45" s="49"/>
       <c r="J45" s="49">
-        <f>SUM(J32:J38)</f>
-        <v>238000</v>
+        <f>SUM(J32:J39)</f>
+        <v>272000</v>
       </c>
       <c r="K45" s="49"/>
       <c r="L45" s="49"/>
       <c r="M45" s="49"/>
       <c r="N45" s="49">
-        <f>SUM(N32:N38)</f>
+        <f>SUM(N32:N39)</f>
         <v>235000</v>
       </c>
       <c r="O45" s="49"/>
       <c r="P45" s="49">
-        <f>SUM(P32:P44) - P36</f>
-        <v>36220.9</v>
+        <f>SUM(P32:P44) - P39</f>
+        <v>42610.900000000009</v>
       </c>
       <c r="Q45" s="50">
-        <f xml:space="preserve"> Q38</f>
-        <v>126919</v>
+        <f xml:space="preserve"> Q39</f>
+        <v>105610.9</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
@@ -2198,12 +2239,12 @@
       <c r="F47" s="30"/>
     </row>
     <row r="51" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G51" s="68" t="s">
+      <c r="G51" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="H51" s="69"/>
-      <c r="I51" s="69"/>
-      <c r="J51" s="69"/>
+      <c r="H51" s="63"/>
+      <c r="I51" s="63"/>
+      <c r="J51" s="63"/>
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G52" s="13" t="s">
@@ -2266,16 +2307,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="B30:B31"/>
     <mergeCell ref="G51:J51"/>
     <mergeCell ref="N30:N31"/>
     <mergeCell ref="O30:O31"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="P30:P31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -2348,34 +2389,34 @@
       </c>
       <c r="M9" s="31">
         <f ca="1">TODAY()</f>
-        <v>42104</v>
+        <v>42113</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="65" t="s">
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="63" t="s">
+      <c r="J14" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="65" t="s">
+      <c r="K14" s="72"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="65" t="s">
+      <c r="N14" s="64" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="9" t="s">
@@ -2383,7 +2424,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A15" s="74"/>
+      <c r="A15" s="75"/>
       <c r="B15" s="8" t="s">
         <v>3</v>
       </c>
@@ -2405,7 +2446,7 @@
       <c r="H15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="67"/>
+      <c r="I15" s="73"/>
       <c r="J15" s="8" t="s">
         <v>7</v>
       </c>
@@ -2415,8 +2456,8 @@
       <c r="L15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="67"/>
-      <c r="N15" s="75"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="76"/>
       <c r="O15" s="5">
         <v>100000</v>
       </c>
@@ -2627,11 +2668,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="78"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">

</xml_diff>

<commit_message>
9. Hafta Bütçe Güncellemesi
9. Hafta için bütçe güncellemesi yapılmıştır.
</commit_message>
<xml_diff>
--- a/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
+++ b/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>Yazılım Test Uzmanı</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Gereksinim Belgesi</t>
+  </si>
+  <si>
+    <t>Tasarım Belgesi</t>
   </si>
 </sst>
 </file>
@@ -812,10 +815,22 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -824,30 +839,24 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="30"/>
     </xf>
@@ -861,12 +870,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1088,12 +1091,73 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>636494</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="157548" cy="248851"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Metin kutusu 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11806518" y="7360023"/>
+          <a:ext cx="157548" cy="248851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1000" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>4</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" i="1">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tablo8" displayName="Tablo8" ref="G52:J55" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="G52:J55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tablo8" displayName="Tablo8" ref="G52:J56" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="G52:J56"/>
   <tableColumns count="4">
     <tableColumn id="1" name="NO" dataDxfId="3"/>
     <tableColumn id="4" name="TARİH" dataDxfId="2">
@@ -1396,10 +1460,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:Q55"/>
+  <dimension ref="A3:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,16 +1515,16 @@
         <v>31</v>
       </c>
       <c r="N9" s="31">
-        <f>DATE(2015,4,17)</f>
-        <v>42111</v>
+        <f>DATE(2015,4,24)</f>
+        <v>42118</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="H17" s="66" t="s">
+      <c r="H17" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="67"/>
-      <c r="J17" s="68"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="75"/>
     </row>
     <row r="18" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="H18" s="45" t="s">
@@ -1540,36 +1604,36 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="69" t="s">
+      <c r="A30" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="71" t="s">
+      <c r="C30" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="64" t="s">
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="71" t="s">
+      <c r="K30" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="L30" s="72"/>
-      <c r="M30" s="72"/>
-      <c r="N30" s="64" t="s">
+      <c r="L30" s="67"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="O30" s="64" t="s">
+      <c r="O30" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="P30" s="64" t="s">
+      <c r="P30" s="68" t="s">
         <v>35</v>
       </c>
       <c r="Q30" s="9" t="s">
@@ -1577,8 +1641,8 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="70"/>
-      <c r="B31" s="73"/>
+      <c r="A31" s="65"/>
+      <c r="B31" s="70"/>
       <c r="C31" s="8" t="s">
         <v>3</v>
       </c>
@@ -1600,7 +1664,7 @@
       <c r="I31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="65"/>
+      <c r="J31" s="69"/>
       <c r="K31" s="8" t="s">
         <v>7</v>
       </c>
@@ -1610,9 +1674,9 @@
       <c r="M31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="65"/>
-      <c r="O31" s="65"/>
-      <c r="P31" s="65"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
       <c r="Q31" s="5">
         <v>100000</v>
       </c>
@@ -1646,7 +1710,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" ref="J32:J39" si="0">SUM(C32:I32)</f>
+        <f t="shared" ref="J32:J40" si="0">SUM(C32:I32)</f>
         <v>34000</v>
       </c>
       <c r="K32" s="3">
@@ -2007,7 +2071,7 @@
         <f xml:space="preserve"> ( (M38 * L38) * K38 / 100 ) + K38</f>
         <v>0</v>
       </c>
-      <c r="O38" s="79">
+      <c r="O38" s="62">
         <f>N38 - J38</f>
         <v>-34000</v>
       </c>
@@ -2065,7 +2129,7 @@
         <f xml:space="preserve"> ( (M39 * L39) * K39 / 100 ) + K39</f>
         <v>0</v>
       </c>
-      <c r="O39" s="80">
+      <c r="O39" s="63">
         <f>N39 - J39</f>
         <v>-34000</v>
       </c>
@@ -2085,21 +2149,56 @@
       <c r="B40" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="6"/>
+      <c r="C40" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D40" s="3">
+        <v>6000</v>
+      </c>
+      <c r="E40" s="3">
+        <v>6000</v>
+      </c>
+      <c r="F40" s="3">
+        <v>4000</v>
+      </c>
+      <c r="G40" s="3">
+        <v>4000</v>
+      </c>
+      <c r="H40" s="3">
+        <v>4000</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
+      <c r="J40" s="3">
+        <f t="shared" si="0"/>
+        <v>34000</v>
+      </c>
+      <c r="K40" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L40" s="3">
+        <v>0</v>
+      </c>
+      <c r="M40" s="3">
+        <v>0</v>
+      </c>
+      <c r="N40" s="3">
+        <f xml:space="preserve"> ( (M40 * L40) * K40 / 100 ) + K40</f>
+        <v>100000</v>
+      </c>
+      <c r="O40" s="3">
+        <f>N40 - J40</f>
+        <v>66000</v>
+      </c>
+      <c r="P40" s="3">
+        <f>Q40 * 0.1</f>
+        <v>18217.199000000001</v>
+      </c>
+      <c r="Q40" s="6">
+        <f xml:space="preserve"> (Q39 + O40) + P39</f>
+        <v>182171.99</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
@@ -2206,24 +2305,24 @@
       <c r="H45" s="49"/>
       <c r="I45" s="49"/>
       <c r="J45" s="49">
-        <f>SUM(J32:J39)</f>
-        <v>272000</v>
+        <f>SUM(J32:J40)</f>
+        <v>306000</v>
       </c>
       <c r="K45" s="49"/>
       <c r="L45" s="49"/>
       <c r="M45" s="49"/>
       <c r="N45" s="49">
-        <f>SUM(N32:N39)</f>
-        <v>235000</v>
+        <f>SUM(N32:N40)</f>
+        <v>335000</v>
       </c>
       <c r="O45" s="49"/>
       <c r="P45" s="49">
         <f>SUM(P32:P44) - P39</f>
-        <v>42610.900000000009</v>
+        <v>60828.099000000017</v>
       </c>
       <c r="Q45" s="50">
-        <f xml:space="preserve"> Q39</f>
-        <v>105610.9</v>
+        <f xml:space="preserve"> Q40</f>
+        <v>182171.99</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
@@ -2239,12 +2338,12 @@
       <c r="F47" s="30"/>
     </row>
     <row r="51" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G51" s="62" t="s">
+      <c r="G51" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="H51" s="63"/>
-      <c r="I51" s="63"/>
-      <c r="J51" s="63"/>
+      <c r="H51" s="72"/>
+      <c r="I51" s="72"/>
+      <c r="J51" s="72"/>
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G52" s="13" t="s">
@@ -2305,18 +2404,32 @@
         <v>54</v>
       </c>
     </row>
+    <row r="56" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G56" s="13">
+        <v>4</v>
+      </c>
+      <c r="H56" s="56">
+        <v>42118</v>
+      </c>
+      <c r="I56" s="13">
+        <v>9</v>
+      </c>
+      <c r="J56" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="P30:P31"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="C30:I30"/>
     <mergeCell ref="J30:J31"/>
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="P30:P31"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -2389,34 +2502,34 @@
       </c>
       <c r="M9" s="31">
         <f ca="1">TODAY()</f>
-        <v>42113</v>
+        <v>42118</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="64" t="s">
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="71" t="s">
+      <c r="J14" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="64" t="s">
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="64" t="s">
+      <c r="N14" s="68" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="9" t="s">
@@ -2424,7 +2537,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A15" s="75"/>
+      <c r="A15" s="77"/>
       <c r="B15" s="8" t="s">
         <v>3</v>
       </c>
@@ -2446,7 +2559,7 @@
       <c r="H15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="73"/>
+      <c r="I15" s="70"/>
       <c r="J15" s="8" t="s">
         <v>7</v>
       </c>
@@ -2456,8 +2569,8 @@
       <c r="L15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="73"/>
-      <c r="N15" s="76"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="78"/>
       <c r="O15" s="5">
         <v>100000</v>
       </c>
@@ -2668,11 +2781,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="78"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">

</xml_diff>

<commit_message>
10. Hafta Bütçe Güncellemesi
10. hafta için bütçe güncellemesi yapılmıştır.
</commit_message>
<xml_diff>
--- a/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
+++ b/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
@@ -821,6 +821,27 @@
     <xf numFmtId="3" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
@@ -833,29 +854,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="30"/>
@@ -1462,8 +1462,8 @@
   </sheetPr>
   <dimension ref="A3:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,16 +1515,16 @@
         <v>31</v>
       </c>
       <c r="N9" s="31">
-        <f>DATE(2015,4,24)</f>
-        <v>42118</v>
+        <f>DATE(2015,5,1)</f>
+        <v>42125</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="H17" s="73" t="s">
+      <c r="H17" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="74"/>
-      <c r="J17" s="75"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="70"/>
     </row>
     <row r="18" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="H18" s="45" t="s">
@@ -1604,36 +1604,36 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="64" t="s">
+      <c r="A30" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="68" t="s">
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="66" t="s">
+      <c r="K30" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="L30" s="67"/>
-      <c r="M30" s="67"/>
-      <c r="N30" s="68" t="s">
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="O30" s="68" t="s">
+      <c r="O30" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="P30" s="68" t="s">
+      <c r="P30" s="66" t="s">
         <v>35</v>
       </c>
       <c r="Q30" s="9" t="s">
@@ -1641,8 +1641,8 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="65"/>
-      <c r="B31" s="70"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="75"/>
       <c r="C31" s="8" t="s">
         <v>3</v>
       </c>
@@ -1664,7 +1664,7 @@
       <c r="I31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="69"/>
+      <c r="J31" s="67"/>
       <c r="K31" s="8" t="s">
         <v>7</v>
       </c>
@@ -1674,9 +1674,9 @@
       <c r="M31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="69"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="69"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="67"/>
       <c r="Q31" s="5">
         <v>100000</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" ref="J32:J40" si="0">SUM(C32:I32)</f>
+        <f t="shared" ref="J32:J41" si="0">SUM(C32:I32)</f>
         <v>34000</v>
       </c>
       <c r="K32" s="3">
@@ -1902,7 +1902,7 @@
         <v>26000</v>
       </c>
       <c r="P35" s="4">
-        <f>Q35 * 0.1</f>
+        <f t="shared" ref="P35:P41" si="1">Q35 * 0.1</f>
         <v>8900</v>
       </c>
       <c r="Q35" s="7">
@@ -1960,7 +1960,7 @@
         <v>-34000</v>
       </c>
       <c r="P36" s="3">
-        <f>Q36 * 0.1</f>
+        <f t="shared" si="1"/>
         <v>6390</v>
       </c>
       <c r="Q36" s="6">
@@ -2018,7 +2018,7 @@
         <v>76000</v>
       </c>
       <c r="P37" s="4">
-        <f>Q37 * 0.1</f>
+        <f t="shared" si="1"/>
         <v>14629</v>
       </c>
       <c r="Q37" s="7">
@@ -2076,7 +2076,7 @@
         <v>-34000</v>
       </c>
       <c r="P38" s="11">
-        <f>Q38 * 0.1</f>
+        <f t="shared" si="1"/>
         <v>12691.900000000001</v>
       </c>
       <c r="Q38" s="61">
@@ -2134,7 +2134,7 @@
         <v>-34000</v>
       </c>
       <c r="P39" s="52">
-        <f>Q39 * 0.1</f>
+        <f t="shared" si="1"/>
         <v>10561.09</v>
       </c>
       <c r="Q39" s="53">
@@ -2187,12 +2187,12 @@
         <f xml:space="preserve"> ( (M40 * L40) * K40 / 100 ) + K40</f>
         <v>100000</v>
       </c>
-      <c r="O40" s="3">
+      <c r="O40" s="54">
         <f>N40 - J40</f>
         <v>66000</v>
       </c>
       <c r="P40" s="3">
-        <f>Q40 * 0.1</f>
+        <f t="shared" si="1"/>
         <v>18217.199000000001</v>
       </c>
       <c r="Q40" s="6">
@@ -2207,21 +2207,56 @@
       <c r="B41" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="7"/>
+      <c r="C41" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D41" s="4">
+        <v>6000</v>
+      </c>
+      <c r="E41" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F41" s="4">
+        <v>4000</v>
+      </c>
+      <c r="G41" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H41" s="4">
+        <v>4000</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
+      <c r="J41" s="4">
+        <f t="shared" si="0"/>
+        <v>34000</v>
+      </c>
+      <c r="K41" s="4">
+        <v>0</v>
+      </c>
+      <c r="L41" s="4">
+        <v>0</v>
+      </c>
+      <c r="M41" s="4">
+        <v>0</v>
+      </c>
+      <c r="N41" s="4">
+        <f xml:space="preserve"> ( (M41 * L41) * K41 / 100 ) + K41</f>
+        <v>0</v>
+      </c>
+      <c r="O41" s="55">
+        <f>N41 - J41</f>
+        <v>-34000</v>
+      </c>
+      <c r="P41" s="4">
+        <f t="shared" si="1"/>
+        <v>16638.918900000001</v>
+      </c>
+      <c r="Q41" s="7">
+        <f xml:space="preserve"> (Q40 + O41) + P40</f>
+        <v>166389.18899999998</v>
+      </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
@@ -2305,24 +2340,24 @@
       <c r="H45" s="49"/>
       <c r="I45" s="49"/>
       <c r="J45" s="49">
-        <f>SUM(J32:J40)</f>
-        <v>306000</v>
+        <f>SUM(J32:J41)</f>
+        <v>340000</v>
       </c>
       <c r="K45" s="49"/>
       <c r="L45" s="49"/>
       <c r="M45" s="49"/>
       <c r="N45" s="49">
-        <f>SUM(N32:N40)</f>
+        <f>SUM(N32:N41)</f>
         <v>335000</v>
       </c>
       <c r="O45" s="49"/>
       <c r="P45" s="49">
         <f>SUM(P32:P44) - P39</f>
-        <v>60828.099000000017</v>
+        <v>77467.017900000021</v>
       </c>
       <c r="Q45" s="50">
-        <f xml:space="preserve"> Q40</f>
-        <v>182171.99</v>
+        <f xml:space="preserve"> Q41</f>
+        <v>166389.18899999998</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
@@ -2338,12 +2373,12 @@
       <c r="F47" s="30"/>
     </row>
     <row r="51" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G51" s="71" t="s">
+      <c r="G51" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72"/>
+      <c r="H51" s="65"/>
+      <c r="I51" s="65"/>
+      <c r="J51" s="65"/>
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G52" s="13" t="s">
@@ -2379,7 +2414,7 @@
         <v>2</v>
       </c>
       <c r="H54" s="56">
-        <f t="shared" ref="H54" si="1">DATE(2015,3,18)</f>
+        <f t="shared" ref="H54" si="2">DATE(2015,3,18)</f>
         <v>42081</v>
       </c>
       <c r="I54" s="13">
@@ -2420,16 +2455,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="B30:B31"/>
     <mergeCell ref="G51:J51"/>
     <mergeCell ref="N30:N31"/>
     <mergeCell ref="O30:O31"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="P30:P31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -2502,34 +2537,34 @@
       </c>
       <c r="M9" s="31">
         <f ca="1">TODAY()</f>
-        <v>42118</v>
+        <v>42127</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68" t="s">
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="66" t="s">
+      <c r="J14" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="68" t="s">
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="68" t="s">
+      <c r="N14" s="66" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="9" t="s">
@@ -2559,7 +2594,7 @@
       <c r="H15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="70"/>
+      <c r="I15" s="75"/>
       <c r="J15" s="8" t="s">
         <v>7</v>
       </c>
@@ -2569,7 +2604,7 @@
       <c r="L15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="70"/>
+      <c r="M15" s="75"/>
       <c r="N15" s="78"/>
       <c r="O15" s="5">
         <v>100000</v>
@@ -2784,7 +2819,7 @@
       <c r="A1" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="67"/>
+      <c r="B1" s="74"/>
       <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
11. Hafta Bütçe Güncellemesi
11. Hafta için bütçe güncellemesi yapılmıştır.
</commit_message>
<xml_diff>
--- a/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
+++ b/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="BBM487-20142-1 Bilgilendirme" sheetId="3" r:id="rId1"/>
-    <sheet name="BBM487-20142-1 Bütçe" sheetId="1" r:id="rId2"/>
-    <sheet name="Grup Üye ve Görevleri" sheetId="2" r:id="rId3"/>
+    <sheet name="Grup Üye ve Görevleri" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Yazılım Test Uzmanı</t>
   </si>
@@ -102,13 +101,7 @@
     <t>İSİM</t>
   </si>
   <si>
-    <t>1. GRUP BÜTÇE TABLOSU</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOT: </t>
-  </si>
-  <si>
-    <t>Bütçedeki Gelir ve Gider Bölümleri her haftanın Cuma günü işlenmektedir.</t>
   </si>
   <si>
     <t xml:space="preserve">Tarih : </t>
@@ -638,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -821,10 +814,16 @@
     <xf numFmtId="3" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,38 +832,23 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1462,8 +1446,8 @@
   </sheetPr>
   <dimension ref="A3:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q46" sqref="Q46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1490,7 +1474,7 @@
     <row r="3" spans="8:14" ht="19.8" x14ac:dyDescent="0.4">
       <c r="H3" s="27"/>
       <c r="I3" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J3" s="28"/>
       <c r="K3" s="13"/>
@@ -1498,7 +1482,7 @@
     <row r="4" spans="8:14" ht="19.8" x14ac:dyDescent="0.4">
       <c r="H4" s="28"/>
       <c r="I4" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="28"/>
     </row>
@@ -1512,19 +1496,19 @@
     </row>
     <row r="9" spans="8:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="M9" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N9" s="31">
-        <f>DATE(2015,5,1)</f>
-        <v>42125</v>
+        <f>DATE(2015,5,8)</f>
+        <v>42132</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="H17" s="68" t="s">
+      <c r="H17" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="69"/>
-      <c r="J17" s="70"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="75"/>
     </row>
     <row r="18" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="H18" s="45" t="s">
@@ -1604,45 +1588,45 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="71" t="s">
+      <c r="A30" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="73" t="s">
+      <c r="B30" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="66" t="s">
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="73" t="s">
+      <c r="K30" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="L30" s="74"/>
-      <c r="M30" s="74"/>
-      <c r="N30" s="66" t="s">
+      <c r="L30" s="67"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="O30" s="66" t="s">
+      <c r="O30" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="P30" s="66" t="s">
-        <v>35</v>
+      <c r="P30" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="Q30" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="72"/>
-      <c r="B31" s="75"/>
+      <c r="A31" s="65"/>
+      <c r="B31" s="70"/>
       <c r="C31" s="8" t="s">
         <v>3</v>
       </c>
@@ -1664,7 +1648,7 @@
       <c r="I31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="67"/>
+      <c r="J31" s="69"/>
       <c r="K31" s="8" t="s">
         <v>7</v>
       </c>
@@ -1674,9 +1658,9 @@
       <c r="M31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="67"/>
-      <c r="O31" s="67"/>
-      <c r="P31" s="67"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
       <c r="Q31" s="5">
         <v>100000</v>
       </c>
@@ -1686,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="57" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C32" s="3">
         <v>10000</v>
@@ -1710,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" ref="J32:J41" si="0">SUM(C32:I32)</f>
+        <f t="shared" ref="J32:J42" si="0">SUM(C32:I32)</f>
         <v>34000</v>
       </c>
       <c r="K32" s="3">
@@ -1743,7 +1727,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C33" s="4">
         <v>10000</v>
@@ -1800,7 +1784,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C34" s="3">
         <v>10000</v>
@@ -1857,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="58" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="4">
         <v>10000</v>
@@ -1915,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="57" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" s="3">
         <v>10000</v>
@@ -1956,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="54">
-        <f>N36 - J36</f>
+        <f t="shared" ref="O36:O42" si="2">N36 - J36</f>
         <v>-34000</v>
       </c>
       <c r="P36" s="3">
@@ -1964,7 +1948,7 @@
         <v>6390</v>
       </c>
       <c r="Q36" s="6">
-        <f xml:space="preserve"> (Q35 + O36) + P35</f>
+        <f t="shared" ref="Q36:Q41" si="3" xml:space="preserve"> (Q35 + O36) + P35</f>
         <v>63900</v>
       </c>
     </row>
@@ -1973,7 +1957,7 @@
         <v>6</v>
       </c>
       <c r="B37" s="58" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" s="4">
         <v>10000</v>
@@ -2014,7 +1998,7 @@
         <v>110000</v>
       </c>
       <c r="O37" s="55">
-        <f>N37 - J37</f>
+        <f t="shared" si="2"/>
         <v>76000</v>
       </c>
       <c r="P37" s="4">
@@ -2022,7 +2006,7 @@
         <v>14629</v>
       </c>
       <c r="Q37" s="7">
-        <f xml:space="preserve"> (Q36 + O37) + P36</f>
+        <f t="shared" si="3"/>
         <v>146290</v>
       </c>
     </row>
@@ -2031,7 +2015,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" s="11">
         <v>10000</v>
@@ -2072,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="O38" s="62">
-        <f>N38 - J38</f>
+        <f t="shared" si="2"/>
         <v>-34000</v>
       </c>
       <c r="P38" s="11">
@@ -2080,7 +2064,7 @@
         <v>12691.900000000001</v>
       </c>
       <c r="Q38" s="61">
-        <f xml:space="preserve"> (Q37 + O38) + P37</f>
+        <f t="shared" si="3"/>
         <v>126919</v>
       </c>
     </row>
@@ -2089,7 +2073,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C39" s="52">
         <v>10000</v>
@@ -2130,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="O39" s="63">
-        <f>N39 - J39</f>
+        <f t="shared" si="2"/>
         <v>-34000</v>
       </c>
       <c r="P39" s="52">
@@ -2138,7 +2122,7 @@
         <v>10561.09</v>
       </c>
       <c r="Q39" s="53">
-        <f xml:space="preserve"> (Q38 + O39) + P38</f>
+        <f t="shared" si="3"/>
         <v>105610.9</v>
       </c>
     </row>
@@ -2147,7 +2131,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="57" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" s="3">
         <v>10000</v>
@@ -2188,7 +2172,7 @@
         <v>100000</v>
       </c>
       <c r="O40" s="54">
-        <f>N40 - J40</f>
+        <f t="shared" si="2"/>
         <v>66000</v>
       </c>
       <c r="P40" s="3">
@@ -2196,7 +2180,7 @@
         <v>18217.199000000001</v>
       </c>
       <c r="Q40" s="6">
-        <f xml:space="preserve"> (Q39 + O40) + P39</f>
+        <f t="shared" si="3"/>
         <v>182171.99</v>
       </c>
     </row>
@@ -2205,7 +2189,7 @@
         <v>10</v>
       </c>
       <c r="B41" s="59" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" s="4">
         <v>10000</v>
@@ -2246,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="O41" s="55">
-        <f>N41 - J41</f>
+        <f t="shared" si="2"/>
         <v>-34000</v>
       </c>
       <c r="P41" s="4">
@@ -2254,7 +2238,7 @@
         <v>16638.918900000001</v>
       </c>
       <c r="Q41" s="7">
-        <f xml:space="preserve"> (Q40 + O41) + P40</f>
+        <f t="shared" si="3"/>
         <v>166389.18899999998</v>
       </c>
     </row>
@@ -2263,30 +2247,65 @@
         <v>11</v>
       </c>
       <c r="B42" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="C42" s="11">
+        <v>10000</v>
+      </c>
+      <c r="D42" s="11">
+        <v>6000</v>
+      </c>
+      <c r="E42" s="11">
+        <v>6000</v>
+      </c>
+      <c r="F42" s="11">
+        <v>4000</v>
+      </c>
+      <c r="G42" s="11">
+        <v>4000</v>
+      </c>
+      <c r="H42" s="11">
+        <v>4000</v>
+      </c>
+      <c r="I42" s="11">
+        <v>0</v>
+      </c>
+      <c r="J42" s="11">
+        <f t="shared" si="0"/>
+        <v>34000</v>
+      </c>
+      <c r="K42" s="11">
+        <v>0</v>
+      </c>
+      <c r="L42" s="11">
+        <v>0</v>
+      </c>
+      <c r="M42" s="11">
+        <v>0</v>
+      </c>
+      <c r="N42" s="11">
+        <f xml:space="preserve"> ( (M42 * L42) * K42 / 100 ) + K42</f>
+        <v>0</v>
+      </c>
+      <c r="O42" s="62">
+        <f t="shared" si="2"/>
+        <v>-34000</v>
+      </c>
+      <c r="P42" s="11">
+        <f>Q42 * 0.1</f>
+        <v>14902.810789999998</v>
+      </c>
+      <c r="Q42" s="61">
+        <f xml:space="preserve"> (Q41 + O42) + P41</f>
+        <v>149028.10789999997</v>
+      </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>12</v>
       </c>
       <c r="B43" s="58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2309,7 +2328,7 @@
         <v>13</v>
       </c>
       <c r="B44" s="57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
@@ -2340,58 +2359,58 @@
       <c r="H45" s="49"/>
       <c r="I45" s="49"/>
       <c r="J45" s="49">
-        <f>SUM(J32:J41)</f>
-        <v>340000</v>
+        <f>SUM(J32:J42)</f>
+        <v>374000</v>
       </c>
       <c r="K45" s="49"/>
       <c r="L45" s="49"/>
       <c r="M45" s="49"/>
       <c r="N45" s="49">
-        <f>SUM(N32:N41)</f>
+        <f>SUM(N32:N42)</f>
         <v>335000</v>
       </c>
       <c r="O45" s="49"/>
       <c r="P45" s="49">
-        <f>SUM(P32:P44) - P39</f>
-        <v>77467.017900000021</v>
+        <f>SUM(P32:P44) - P342</f>
+        <v>102930.91869000002</v>
       </c>
       <c r="Q45" s="50">
-        <f xml:space="preserve"> Q41</f>
-        <v>166389.18899999998</v>
+        <f xml:space="preserve"> Q42</f>
+        <v>149028.10789999997</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="29"/>
       <c r="C47" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30"/>
       <c r="F47" s="30"/>
     </row>
     <row r="51" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G51" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="H51" s="65"/>
-      <c r="I51" s="65"/>
-      <c r="J51" s="65"/>
+      <c r="G51" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="H51" s="72"/>
+      <c r="I51" s="72"/>
+      <c r="J51" s="72"/>
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G52" s="13" t="s">
         <v>25</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>13</v>
       </c>
       <c r="J52" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="7:10" x14ac:dyDescent="0.3">
@@ -2406,7 +2425,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="7:10" x14ac:dyDescent="0.3">
@@ -2414,14 +2433,14 @@
         <v>2</v>
       </c>
       <c r="H54" s="56">
-        <f t="shared" ref="H54" si="2">DATE(2015,3,18)</f>
+        <f t="shared" ref="H54" si="4">DATE(2015,3,18)</f>
         <v>42081</v>
       </c>
       <c r="I54" s="13">
         <v>4</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="7:10" x14ac:dyDescent="0.3">
@@ -2436,7 +2455,7 @@
         <v>6</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="7:10" x14ac:dyDescent="0.3">
@@ -2450,21 +2469,21 @@
         <v>9</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="P30:P31"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="C30:I30"/>
     <mergeCell ref="J30:J31"/>
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="P30:P31"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -2480,328 +2499,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A3:O25"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:K4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" customWidth="1"/>
-    <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:15" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="G3" s="27"/>
-      <c r="H3" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:15" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="G4" s="28"/>
-      <c r="H4" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L6" s="14"/>
-      <c r="M6" s="25"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L7" s="25"/>
-      <c r="M7" s="26"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L9" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="31">
-        <f ca="1">TODAY()</f>
-        <v>42127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
-      <c r="M14" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="N14" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A15" s="77"/>
-      <c r="B15" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="75"/>
-      <c r="J15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="M15" s="75"/>
-      <c r="N15" s="78"/>
-      <c r="O15" s="5">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3">
-        <v>10000</v>
-      </c>
-      <c r="C16" s="3">
-        <v>6000</v>
-      </c>
-      <c r="D16" s="3">
-        <v>6000</v>
-      </c>
-      <c r="E16" s="3">
-        <v>4000</v>
-      </c>
-      <c r="F16" s="3">
-        <v>4000</v>
-      </c>
-      <c r="G16" s="3">
-        <v>4000</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0</v>
-      </c>
-      <c r="I16" s="3">
-        <f>SUM(B16:H16)</f>
-        <v>34000</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0</v>
-      </c>
-      <c r="L16" s="3">
-        <v>0</v>
-      </c>
-      <c r="M16" s="3">
-        <f xml:space="preserve"> (L16 * K16) * J16 / 100</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="3">
-        <f xml:space="preserve"> (M16-I16)</f>
-        <v>-34000</v>
-      </c>
-      <c r="O16" s="6">
-        <f xml:space="preserve"> (O15 + N16)</f>
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>2</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="7"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="6"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>4</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="7"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>5</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="6"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>6</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="7"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
-        <v>7</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="12"/>
-    </row>
-    <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="M14:M15"/>
-  </mergeCells>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="60" orientation="landscape" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2816,11 +2513,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">

</xml_diff>

<commit_message>
12. Hafta Bütçe Güncellemesi
12. Hafta için Bütçe Güncellemesinin Yapılması
</commit_message>
<xml_diff>
--- a/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
+++ b/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
@@ -814,6 +814,27 @@
     <xf numFmtId="3" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
@@ -826,29 +847,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1446,7 +1446,7 @@
   </sheetPr>
   <dimension ref="A3:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -1499,16 +1499,16 @@
         <v>29</v>
       </c>
       <c r="N9" s="31">
-        <f>DATE(2015,5,8)</f>
-        <v>42132</v>
+        <f>DATE(2015,5,15)</f>
+        <v>42139</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="H17" s="73" t="s">
+      <c r="H17" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="74"/>
-      <c r="J17" s="75"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="70"/>
     </row>
     <row r="18" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="H18" s="45" t="s">
@@ -1588,36 +1588,36 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="64" t="s">
+      <c r="A30" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="68" t="s">
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="66" t="s">
+      <c r="K30" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="L30" s="67"/>
-      <c r="M30" s="67"/>
-      <c r="N30" s="68" t="s">
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="O30" s="68" t="s">
+      <c r="O30" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="P30" s="68" t="s">
+      <c r="P30" s="66" t="s">
         <v>33</v>
       </c>
       <c r="Q30" s="9" t="s">
@@ -1625,8 +1625,8 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="65"/>
-      <c r="B31" s="70"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="75"/>
       <c r="C31" s="8" t="s">
         <v>3</v>
       </c>
@@ -1648,7 +1648,7 @@
       <c r="I31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="69"/>
+      <c r="J31" s="67"/>
       <c r="K31" s="8" t="s">
         <v>7</v>
       </c>
@@ -1658,9 +1658,9 @@
       <c r="M31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="69"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="69"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="67"/>
       <c r="Q31" s="5">
         <v>100000</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" ref="J32:J42" si="0">SUM(C32:I32)</f>
+        <f t="shared" ref="J32:J43" si="0">SUM(C32:I32)</f>
         <v>34000</v>
       </c>
       <c r="K32" s="3">
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="54">
-        <f t="shared" ref="O36:O42" si="2">N36 - J36</f>
+        <f t="shared" ref="O36:O43" si="2">N36 - J36</f>
         <v>-34000</v>
       </c>
       <c r="P36" s="3">
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="N37" s="4">
-        <f xml:space="preserve"> ( (M37 * L37) * K37 / 100 ) + K37</f>
+        <f t="shared" ref="N37:N43" si="4" xml:space="preserve"> ( (M37 * L37) * K37 / 100 ) + K37</f>
         <v>110000</v>
       </c>
       <c r="O37" s="55">
@@ -2052,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="N38" s="11">
-        <f xml:space="preserve"> ( (M38 * L38) * K38 / 100 ) + K38</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O38" s="62">
@@ -2110,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="N39" s="52">
-        <f xml:space="preserve"> ( (M39 * L39) * K39 / 100 ) + K39</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O39" s="63">
@@ -2168,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="N40" s="3">
-        <f xml:space="preserve"> ( (M40 * L40) * K40 / 100 ) + K40</f>
+        <f t="shared" si="4"/>
         <v>100000</v>
       </c>
       <c r="O40" s="54">
@@ -2226,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="N41" s="4">
-        <f xml:space="preserve"> ( (M41 * L41) * K41 / 100 ) + K41</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O41" s="55">
@@ -2284,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="N42" s="11">
-        <f xml:space="preserve"> ( (M42 * L42) * K42 / 100 ) + K42</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O42" s="62">
@@ -2307,21 +2307,56 @@
       <c r="B43" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="7"/>
+      <c r="C43" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D43" s="4">
+        <v>6000</v>
+      </c>
+      <c r="E43" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F43" s="4">
+        <v>4000</v>
+      </c>
+      <c r="G43" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H43" s="4">
+        <v>4000</v>
+      </c>
+      <c r="I43" s="4">
+        <v>0</v>
+      </c>
+      <c r="J43" s="4">
+        <f t="shared" si="0"/>
+        <v>34000</v>
+      </c>
+      <c r="K43" s="4">
+        <v>0</v>
+      </c>
+      <c r="L43" s="4">
+        <v>0</v>
+      </c>
+      <c r="M43" s="4">
+        <v>0</v>
+      </c>
+      <c r="N43" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O43" s="4">
+        <f t="shared" si="2"/>
+        <v>-34000</v>
+      </c>
+      <c r="P43" s="4">
+        <f>Q43 * 0.1</f>
+        <v>12993.091868999998</v>
+      </c>
+      <c r="Q43" s="7">
+        <f xml:space="preserve"> (Q42 + O43) + P42</f>
+        <v>129930.91868999998</v>
+      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="10">
@@ -2359,24 +2394,24 @@
       <c r="H45" s="49"/>
       <c r="I45" s="49"/>
       <c r="J45" s="49">
-        <f>SUM(J32:J42)</f>
-        <v>374000</v>
+        <f>SUM(J32:J43)</f>
+        <v>408000</v>
       </c>
       <c r="K45" s="49"/>
       <c r="L45" s="49"/>
       <c r="M45" s="49"/>
       <c r="N45" s="49">
-        <f>SUM(N32:N42)</f>
+        <f>SUM(N32:N43)</f>
         <v>335000</v>
       </c>
       <c r="O45" s="49"/>
       <c r="P45" s="49">
-        <f>SUM(P32:P44) - P342</f>
+        <f>SUM(P32:P44) - P43</f>
         <v>102930.91869000002</v>
       </c>
       <c r="Q45" s="50">
-        <f xml:space="preserve"> Q42</f>
-        <v>149028.10789999997</v>
+        <f xml:space="preserve"> Q43</f>
+        <v>129930.91868999998</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
@@ -2392,12 +2427,12 @@
       <c r="F47" s="30"/>
     </row>
     <row r="51" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G51" s="71" t="s">
+      <c r="G51" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72"/>
+      <c r="H51" s="65"/>
+      <c r="I51" s="65"/>
+      <c r="J51" s="65"/>
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G52" s="13" t="s">
@@ -2433,7 +2468,7 @@
         <v>2</v>
       </c>
       <c r="H54" s="56">
-        <f t="shared" ref="H54" si="4">DATE(2015,3,18)</f>
+        <f t="shared" ref="H54" si="5">DATE(2015,3,18)</f>
         <v>42081</v>
       </c>
       <c r="I54" s="13">
@@ -2474,16 +2509,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="B30:B31"/>
     <mergeCell ref="G51:J51"/>
     <mergeCell ref="N30:N31"/>
     <mergeCell ref="O30:O31"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="P30:P31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -2516,7 +2551,7 @@
       <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="67"/>
+      <c r="B1" s="74"/>
       <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
13. Hafta Bütçe Güncellemesi
13. Hafta için bütçe güncellemesi yapılmıştır.
</commit_message>
<xml_diff>
--- a/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
+++ b/Docs/487_20142_1_Bilgilendirme_Belgesi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>Yazılım Test Uzmanı</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Tasarım Belgesi</t>
+  </si>
+  <si>
+    <t>Son Teslim</t>
   </si>
 </sst>
 </file>
@@ -631,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -664,9 +667,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -814,10 +814,16 @@
     <xf numFmtId="3" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -826,29 +832,23 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="30"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1136,12 +1136,73 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>618564</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>134469</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="157548" cy="248851"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Metin kutusu 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11788588" y="8095128"/>
+          <a:ext cx="157548" cy="248851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1000" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>5</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" i="1">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tablo8" displayName="Tablo8" ref="G52:J56" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="G52:J56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tablo8" displayName="Tablo8" ref="G52:J57" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="G52:J57"/>
   <tableColumns count="4">
     <tableColumn id="1" name="NO" dataDxfId="3"/>
     <tableColumn id="4" name="TARİH" dataDxfId="2">
@@ -1444,10 +1505,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:Q56"/>
+  <dimension ref="A3:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1472,152 +1533,152 @@
   </cols>
   <sheetData>
     <row r="3" spans="8:14" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="H3" s="27"/>
-      <c r="I3" s="28" t="s">
+      <c r="H3" s="26"/>
+      <c r="I3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="13"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="8:14" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="H4" s="28"/>
-      <c r="I4" s="28" t="s">
+      <c r="H4" s="27"/>
+      <c r="I4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="28"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="6" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="M6" s="14"/>
-      <c r="N6" s="25"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="24"/>
     </row>
     <row r="7" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="M7" s="25"/>
-      <c r="N7" s="26"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="25"/>
     </row>
     <row r="9" spans="8:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="31">
-        <f>DATE(2015,5,15)</f>
-        <v>42139</v>
+      <c r="N9" s="30">
+        <f>DATE(2015,5,22)</f>
+        <v>42146</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="H17" s="68" t="s">
+      <c r="H17" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="69"/>
-      <c r="J17" s="70"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="74"/>
     </row>
     <row r="18" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="H18" s="45" t="s">
+      <c r="H18" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="46" t="s">
+      <c r="I18" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="47" t="s">
+      <c r="J18" s="46" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="41" t="s">
+      <c r="I19" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="37">
+      <c r="J19" s="36">
         <v>21127179</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="42" t="s">
+      <c r="I20" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="38">
+      <c r="J20" s="37">
         <v>20826176</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="39">
+      <c r="J21" s="38">
         <v>21228194</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="42" t="s">
+      <c r="I22" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="38">
+      <c r="J22" s="37">
         <v>21383546</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="43" t="s">
+      <c r="I23" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="39">
+      <c r="J23" s="38">
         <v>21127501</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H24" s="36" t="s">
+      <c r="H24" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="44" t="s">
+      <c r="I24" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="40">
+      <c r="J24" s="39">
         <v>21383579</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="71" t="s">
+      <c r="A30" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="73" t="s">
+      <c r="C30" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="66" t="s">
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="73" t="s">
+      <c r="K30" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="L30" s="74"/>
-      <c r="M30" s="74"/>
-      <c r="N30" s="66" t="s">
+      <c r="L30" s="66"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="O30" s="66" t="s">
+      <c r="O30" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="P30" s="66" t="s">
+      <c r="P30" s="67" t="s">
         <v>33</v>
       </c>
       <c r="Q30" s="9" t="s">
@@ -1625,8 +1686,8 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="72"/>
-      <c r="B31" s="75"/>
+      <c r="A31" s="64"/>
+      <c r="B31" s="69"/>
       <c r="C31" s="8" t="s">
         <v>3</v>
       </c>
@@ -1648,7 +1709,7 @@
       <c r="I31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="67"/>
+      <c r="J31" s="68"/>
       <c r="K31" s="8" t="s">
         <v>7</v>
       </c>
@@ -1658,9 +1719,9 @@
       <c r="M31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="67"/>
-      <c r="O31" s="67"/>
-      <c r="P31" s="67"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
       <c r="Q31" s="5">
         <v>100000</v>
       </c>
@@ -1669,7 +1730,7 @@
       <c r="A32" s="2">
         <v>1</v>
       </c>
-      <c r="B32" s="57" t="s">
+      <c r="B32" s="56" t="s">
         <v>50</v>
       </c>
       <c r="C32" s="3">
@@ -1694,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" ref="J32:J43" si="0">SUM(C32:I32)</f>
+        <f t="shared" ref="J32:J44" si="0">SUM(C32:I32)</f>
         <v>34000</v>
       </c>
       <c r="K32" s="3">
@@ -1710,7 +1771,7 @@
         <f>( (M32 * L32) * K32 / 100 ) + K32</f>
         <v>0</v>
       </c>
-      <c r="O32" s="54">
+      <c r="O32" s="53">
         <f xml:space="preserve"> (N32-J32)</f>
         <v>-34000</v>
       </c>
@@ -1726,7 +1787,7 @@
       <c r="A33" s="1">
         <v>2</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="57" t="s">
         <v>49</v>
       </c>
       <c r="C33" s="4">
@@ -1767,7 +1828,7 @@
         <f xml:space="preserve"> ( (M33 * L33) * K33 / 100 ) + K33</f>
         <v>65000</v>
       </c>
-      <c r="O33" s="55">
+      <c r="O33" s="54">
         <f xml:space="preserve"> N33 - J33</f>
         <v>31000</v>
       </c>
@@ -1783,7 +1844,7 @@
       <c r="A34" s="2">
         <v>3</v>
       </c>
-      <c r="B34" s="57" t="s">
+      <c r="B34" s="56" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="3">
@@ -1824,7 +1885,7 @@
         <f xml:space="preserve"> ( (M34 * L34) * K34 / 100 ) + K34</f>
         <v>0</v>
       </c>
-      <c r="O34" s="54">
+      <c r="O34" s="53">
         <f xml:space="preserve"> N34 - J34</f>
         <v>-34000</v>
       </c>
@@ -1840,7 +1901,7 @@
       <c r="A35" s="1">
         <v>4</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="57" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="4">
@@ -1881,7 +1942,7 @@
         <f xml:space="preserve"> ( (M35 * L35) * K35 / 100 ) + K35</f>
         <v>60000</v>
       </c>
-      <c r="O35" s="55">
+      <c r="O35" s="54">
         <f xml:space="preserve"> N35 - J35</f>
         <v>26000</v>
       </c>
@@ -1898,7 +1959,7 @@
       <c r="A36" s="2">
         <v>5</v>
       </c>
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="56" t="s">
         <v>39</v>
       </c>
       <c r="C36" s="3">
@@ -1939,7 +2000,7 @@
         <f>SUM(K36:M36)</f>
         <v>0</v>
       </c>
-      <c r="O36" s="54">
+      <c r="O36" s="53">
         <f t="shared" ref="O36:O43" si="2">N36 - J36</f>
         <v>-34000</v>
       </c>
@@ -1956,7 +2017,7 @@
       <c r="A37" s="1">
         <v>6</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="57" t="s">
         <v>40</v>
       </c>
       <c r="C37" s="4">
@@ -1994,10 +2055,10 @@
         <v>1</v>
       </c>
       <c r="N37" s="4">
-        <f t="shared" ref="N37:N43" si="4" xml:space="preserve"> ( (M37 * L37) * K37 / 100 ) + K37</f>
+        <f t="shared" ref="N37:N44" si="4" xml:space="preserve"> ( (M37 * L37) * K37 / 100 ) + K37</f>
         <v>110000</v>
       </c>
-      <c r="O37" s="55">
+      <c r="O37" s="54">
         <f t="shared" si="2"/>
         <v>76000</v>
       </c>
@@ -2014,7 +2075,7 @@
       <c r="A38" s="10">
         <v>7</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="56" t="s">
         <v>41</v>
       </c>
       <c r="C38" s="11">
@@ -2055,7 +2116,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O38" s="62">
+      <c r="O38" s="61">
         <f t="shared" si="2"/>
         <v>-34000</v>
       </c>
@@ -2063,65 +2124,65 @@
         <f t="shared" si="1"/>
         <v>12691.900000000001</v>
       </c>
-      <c r="Q38" s="61">
+      <c r="Q38" s="60">
         <f t="shared" si="3"/>
         <v>126919</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" s="51">
+      <c r="A39" s="50">
         <v>8</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="B39" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="52">
+      <c r="C39" s="51">
         <v>10000</v>
       </c>
-      <c r="D39" s="52">
+      <c r="D39" s="51">
         <v>6000</v>
       </c>
-      <c r="E39" s="52">
+      <c r="E39" s="51">
         <v>6000</v>
       </c>
-      <c r="F39" s="52">
-        <v>4000</v>
-      </c>
-      <c r="G39" s="52">
-        <v>4000</v>
-      </c>
-      <c r="H39" s="52">
-        <v>4000</v>
-      </c>
-      <c r="I39" s="52">
-        <v>0</v>
-      </c>
-      <c r="J39" s="52">
+      <c r="F39" s="51">
+        <v>4000</v>
+      </c>
+      <c r="G39" s="51">
+        <v>4000</v>
+      </c>
+      <c r="H39" s="51">
+        <v>4000</v>
+      </c>
+      <c r="I39" s="51">
+        <v>0</v>
+      </c>
+      <c r="J39" s="51">
         <f t="shared" si="0"/>
         <v>34000</v>
       </c>
-      <c r="K39" s="52">
-        <v>0</v>
-      </c>
-      <c r="L39" s="52">
-        <v>0</v>
-      </c>
-      <c r="M39" s="52">
-        <v>0</v>
-      </c>
-      <c r="N39" s="52">
+      <c r="K39" s="51">
+        <v>0</v>
+      </c>
+      <c r="L39" s="51">
+        <v>0</v>
+      </c>
+      <c r="M39" s="51">
+        <v>0</v>
+      </c>
+      <c r="N39" s="51">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O39" s="63">
+      <c r="O39" s="62">
         <f t="shared" si="2"/>
         <v>-34000</v>
       </c>
-      <c r="P39" s="52">
+      <c r="P39" s="51">
         <f t="shared" si="1"/>
         <v>10561.09</v>
       </c>
-      <c r="Q39" s="53">
+      <c r="Q39" s="52">
         <f t="shared" si="3"/>
         <v>105610.9</v>
       </c>
@@ -2130,7 +2191,7 @@
       <c r="A40" s="2">
         <v>9</v>
       </c>
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="56" t="s">
         <v>43</v>
       </c>
       <c r="C40" s="3">
@@ -2171,7 +2232,7 @@
         <f t="shared" si="4"/>
         <v>100000</v>
       </c>
-      <c r="O40" s="54">
+      <c r="O40" s="53">
         <f t="shared" si="2"/>
         <v>66000</v>
       </c>
@@ -2188,7 +2249,7 @@
       <c r="A41" s="1">
         <v>10</v>
       </c>
-      <c r="B41" s="59" t="s">
+      <c r="B41" s="58" t="s">
         <v>44</v>
       </c>
       <c r="C41" s="4">
@@ -2229,7 +2290,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O41" s="55">
+      <c r="O41" s="54">
         <f t="shared" si="2"/>
         <v>-34000</v>
       </c>
@@ -2246,7 +2307,7 @@
       <c r="A42" s="10">
         <v>11</v>
       </c>
-      <c r="B42" s="57" t="s">
+      <c r="B42" s="56" t="s">
         <v>45</v>
       </c>
       <c r="C42" s="11">
@@ -2287,7 +2348,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O42" s="62">
+      <c r="O42" s="61">
         <f t="shared" si="2"/>
         <v>-34000</v>
       </c>
@@ -2295,7 +2356,7 @@
         <f>Q42 * 0.1</f>
         <v>14902.810789999998</v>
       </c>
-      <c r="Q42" s="61">
+      <c r="Q42" s="60">
         <f xml:space="preserve"> (Q41 + O42) + P41</f>
         <v>149028.10789999997</v>
       </c>
@@ -2304,7 +2365,7 @@
       <c r="A43" s="1">
         <v>12</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="57" t="s">
         <v>46</v>
       </c>
       <c r="C43" s="4">
@@ -2362,163 +2423,213 @@
       <c r="A44" s="10">
         <v>13</v>
       </c>
-      <c r="B44" s="57" t="s">
+      <c r="B44" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="12"/>
+      <c r="C44" s="11">
+        <v>10000</v>
+      </c>
+      <c r="D44" s="11">
+        <v>6000</v>
+      </c>
+      <c r="E44" s="11">
+        <v>6000</v>
+      </c>
+      <c r="F44" s="11">
+        <v>4000</v>
+      </c>
+      <c r="G44" s="11">
+        <v>4000</v>
+      </c>
+      <c r="H44" s="11">
+        <v>4000</v>
+      </c>
+      <c r="I44" s="11">
+        <v>0</v>
+      </c>
+      <c r="J44" s="11">
+        <f t="shared" si="0"/>
+        <v>34000</v>
+      </c>
+      <c r="K44" s="11">
+        <v>100000</v>
+      </c>
+      <c r="L44" s="11">
+        <v>0</v>
+      </c>
+      <c r="M44" s="11">
+        <v>0</v>
+      </c>
+      <c r="N44" s="11">
+        <f t="shared" si="4"/>
+        <v>100000</v>
+      </c>
+      <c r="O44" s="11">
+        <f>N44 - J44</f>
+        <v>66000</v>
+      </c>
+      <c r="P44" s="11">
+        <f>Q44 * 0.1 * 0</f>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="60">
+        <f xml:space="preserve"> (Q43 + O44) + P43</f>
+        <v>208924.01055899996</v>
+      </c>
     </row>
     <row r="45" spans="1:17" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="48" t="s">
+      <c r="A45" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="60"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="49"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="49">
-        <f>SUM(J32:J43)</f>
-        <v>408000</v>
-      </c>
-      <c r="K45" s="49"/>
-      <c r="L45" s="49"/>
-      <c r="M45" s="49"/>
-      <c r="N45" s="49">
-        <f>SUM(N32:N43)</f>
-        <v>335000</v>
-      </c>
-      <c r="O45" s="49"/>
-      <c r="P45" s="49">
-        <f>SUM(P32:P44) - P43</f>
-        <v>102930.91869000002</v>
-      </c>
-      <c r="Q45" s="50">
-        <f xml:space="preserve"> Q43</f>
-        <v>129930.91868999998</v>
+      <c r="B45" s="59"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48">
+        <f>SUM(J32:J44)</f>
+        <v>442000</v>
+      </c>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48">
+        <f>SUM(N32:N44)</f>
+        <v>435000</v>
+      </c>
+      <c r="O45" s="48"/>
+      <c r="P45" s="48">
+        <f>SUM(P32:P44) - P44</f>
+        <v>115924.01055900002</v>
+      </c>
+      <c r="Q45" s="49">
+        <f xml:space="preserve"> Q44</f>
+        <v>208924.01055899996</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="30" t="s">
+      <c r="B47" s="28"/>
+      <c r="C47" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
     </row>
     <row r="51" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G51" s="64" t="s">
+      <c r="G51" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="H51" s="65"/>
-      <c r="I51" s="65"/>
-      <c r="J51" s="65"/>
+      <c r="H51" s="71"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="71"/>
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G52" s="13" t="s">
+      <c r="G52" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H52" s="13" t="s">
+      <c r="H52" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I52" s="13" t="s">
+      <c r="I52" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J52" s="13" t="s">
+      <c r="J52" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="53" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G53" s="13">
+      <c r="G53" s="12">
         <v>1</v>
       </c>
-      <c r="H53" s="56">
+      <c r="H53" s="55">
         <f>DATE(2015,3,3)</f>
         <v>42066</v>
       </c>
-      <c r="I53" s="13">
+      <c r="I53" s="12">
         <v>2</v>
       </c>
-      <c r="J53" s="13" t="s">
+      <c r="J53" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="54" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G54" s="13">
+      <c r="G54" s="12">
         <v>2</v>
       </c>
-      <c r="H54" s="56">
+      <c r="H54" s="55">
         <f t="shared" ref="H54" si="5">DATE(2015,3,18)</f>
         <v>42081</v>
       </c>
-      <c r="I54" s="13">
+      <c r="I54" s="12">
         <v>4</v>
       </c>
-      <c r="J54" s="13" t="s">
+      <c r="J54" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G55" s="13">
+      <c r="G55" s="12">
         <v>3</v>
       </c>
-      <c r="H55" s="56">
+      <c r="H55" s="55">
         <f>DATE(2015,4,2)</f>
         <v>42096</v>
       </c>
-      <c r="I55" s="13">
+      <c r="I55" s="12">
         <v>6</v>
       </c>
-      <c r="J55" s="13" t="s">
+      <c r="J55" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="56" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G56" s="13">
+      <c r="G56" s="12">
         <v>4</v>
       </c>
-      <c r="H56" s="56">
+      <c r="H56" s="55">
         <v>42118</v>
       </c>
-      <c r="I56" s="13">
+      <c r="I56" s="12">
         <v>9</v>
       </c>
-      <c r="J56" s="13" t="s">
+      <c r="J56" s="12" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G57" s="12">
+        <v>5</v>
+      </c>
+      <c r="H57" s="55">
+        <f>DATE(2015,5,22)</f>
+        <v>42146</v>
+      </c>
+      <c r="I57" s="12">
+        <v>13</v>
+      </c>
+      <c r="J57" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="P30:P31"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="C30:I30"/>
     <mergeCell ref="J30:J31"/>
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="P30:P31"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -2548,20 +2659,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="76"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2569,10 +2680,10 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <v>21127179</v>
       </c>
     </row>
@@ -2580,10 +2691,10 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <v>20826176</v>
       </c>
     </row>
@@ -2591,10 +2702,10 @@
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <v>21228194</v>
       </c>
     </row>
@@ -2602,10 +2713,10 @@
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="22">
         <v>21383546</v>
       </c>
     </row>
@@ -2613,21 +2724,21 @@
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="20">
         <v>21127501</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>21383579</v>
       </c>
     </row>

</xml_diff>